<commit_message>
Updated Timeline for Prezi
Fixed the typo
</commit_message>
<xml_diff>
--- a/Documentation/Timeline Spring.xlsx
+++ b/Documentation/Timeline Spring.xlsx
@@ -93,9 +93,6 @@
     <t>Final Presentation</t>
   </si>
   <si>
-    <t>Depoloyment</t>
-  </si>
-  <si>
     <t>Team</t>
   </si>
   <si>
@@ -139,6 +136,9 @@
   </si>
   <si>
     <t>Refine Site and Inconsistencies</t>
+  </si>
+  <si>
+    <t>Deployment</t>
   </si>
 </sst>
 </file>
@@ -735,7 +735,7 @@
   <dimension ref="A6:U35"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A10" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -845,7 +845,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="38" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C12" s="27"/>
       <c r="D12" s="27"/>
@@ -868,10 +868,10 @@
     </row>
     <row r="13" spans="1:21" ht="27" customHeight="1">
       <c r="A13" s="24" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B13" s="38" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C13" s="27"/>
       <c r="D13" s="27"/>
@@ -898,7 +898,7 @@
       </c>
       <c r="B14" s="7"/>
       <c r="C14" s="28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D14" s="28"/>
       <c r="E14" s="28"/>
@@ -925,7 +925,7 @@
       </c>
       <c r="B15" s="7"/>
       <c r="C15" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="10"/>
@@ -947,14 +947,14 @@
     </row>
     <row r="16" spans="1:21" ht="27" customHeight="1">
       <c r="A16" s="24" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B16" s="7"/>
       <c r="C16" s="27"/>
       <c r="D16" s="27"/>
       <c r="E16" s="6"/>
       <c r="F16" s="31" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G16" s="9"/>
       <c r="H16" s="27"/>
@@ -973,12 +973,12 @@
     </row>
     <row r="17" spans="1:21" ht="27" customHeight="1">
       <c r="A17" s="24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B17" s="7"/>
       <c r="C17" s="27"/>
       <c r="D17" s="32" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E17" s="32"/>
       <c r="F17" s="32"/>
@@ -1004,7 +1004,7 @@
       </c>
       <c r="B18" s="7"/>
       <c r="C18" s="33" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D18" s="33"/>
       <c r="E18" s="33"/>
@@ -1032,7 +1032,7 @@
       <c r="B19" s="7"/>
       <c r="C19" s="27"/>
       <c r="D19" s="34" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E19" s="34"/>
       <c r="F19" s="34"/>
@@ -1054,11 +1054,11 @@
     </row>
     <row r="20" spans="1:21" ht="27" customHeight="1">
       <c r="A20" s="24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B20" s="7"/>
       <c r="C20" s="35" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D20" s="35"/>
       <c r="E20" s="35"/>
@@ -1081,11 +1081,11 @@
     </row>
     <row r="21" spans="1:21" ht="27" customHeight="1">
       <c r="A21" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B21" s="7"/>
       <c r="C21" s="36" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D21" s="36"/>
       <c r="E21" s="36"/>
@@ -1108,7 +1108,7 @@
     </row>
     <row r="22" spans="1:21" ht="27" customHeight="1">
       <c r="A22" s="24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B22" s="7"/>
       <c r="C22" s="27"/>
@@ -1117,7 +1117,7 @@
       <c r="F22" s="26"/>
       <c r="G22" s="8"/>
       <c r="H22" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I22" s="6"/>
       <c r="J22" s="27"/>
@@ -1145,7 +1145,7 @@
       <c r="G23" s="8"/>
       <c r="H23" s="7"/>
       <c r="I23" s="17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J23" s="27"/>
       <c r="K23" s="27"/>
@@ -1162,7 +1162,7 @@
     </row>
     <row r="24" spans="1:21" ht="27" customHeight="1">
       <c r="A24" s="24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B24" s="7"/>
       <c r="C24" s="27"/>
@@ -1173,7 +1173,7 @@
       <c r="H24" s="7"/>
       <c r="I24" s="6"/>
       <c r="J24" s="37" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K24" s="37"/>
       <c r="L24" s="37"/>
@@ -1200,7 +1200,7 @@
       <c r="H25" s="7"/>
       <c r="I25" s="6"/>
       <c r="J25" s="43" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K25" s="44"/>
       <c r="L25" s="27"/>
@@ -1229,7 +1229,7 @@
       <c r="J26" s="27"/>
       <c r="K26" s="6"/>
       <c r="L26" s="47" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M26" s="48"/>
       <c r="N26" s="27"/>
@@ -1256,7 +1256,7 @@
       <c r="J27" s="27"/>
       <c r="K27" s="6"/>
       <c r="L27" s="47" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M27" s="48"/>
       <c r="N27" s="27"/>
@@ -1285,7 +1285,7 @@
       <c r="L28" s="27"/>
       <c r="M28" s="6"/>
       <c r="N28" s="43" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O28" s="44"/>
       <c r="P28" s="25"/>
@@ -1314,7 +1314,7 @@
       <c r="N29" s="27"/>
       <c r="O29" s="6"/>
       <c r="P29" s="47" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q29" s="48"/>
       <c r="R29" s="27"/>
@@ -1341,7 +1341,7 @@
       <c r="N30" s="27"/>
       <c r="O30" s="6"/>
       <c r="P30" s="47" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q30" s="48"/>
       <c r="R30" s="27"/>
@@ -1368,7 +1368,7 @@
       <c r="N31" s="27"/>
       <c r="O31" s="6"/>
       <c r="P31" s="31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Q31" s="9"/>
       <c r="R31" s="27"/>
@@ -1395,7 +1395,7 @@
       <c r="N32" s="27"/>
       <c r="O32" s="6"/>
       <c r="P32" s="45" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q32" s="46"/>
       <c r="R32" s="27"/>
@@ -1424,7 +1424,7 @@
       <c r="P33" s="27"/>
       <c r="Q33" s="6"/>
       <c r="R33" s="40" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="S33" s="2"/>
       <c r="T33" s="2"/>
@@ -1432,7 +1432,7 @@
     </row>
     <row r="34" spans="1:21" ht="27" customHeight="1">
       <c r="A34" s="24" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="B34" s="7"/>
       <c r="C34" s="27"/>
@@ -1451,7 +1451,7 @@
       <c r="P34" s="27"/>
       <c r="Q34" s="6"/>
       <c r="R34" s="40" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="S34" s="2"/>
       <c r="T34" s="2"/>

</xml_diff>